<commit_message>
NEW FILES ADDED ANS SOME CHANGES
</commit_message>
<xml_diff>
--- a/files/emplyees.xlsx
+++ b/files/emplyees.xlsx
@@ -1,17 +1,5 @@
 
-<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
-  <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
-  </bookViews>
-  <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet_name_1" sheetId="1" state="visible" r:id="rId1"/>
-  </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
-</workbook>
+<file path=xl/workbook.xml><workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"><workbookPr/><workbookProtection/><bookViews><workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/></bookViews><sheets><sheet sheetId="1" state="visible" r:id="rId1" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet_name_1"/><sheet r:id="rId4" name="employees" sheetId="2"/></sheets><definedNames><definedName name="employees">'employees'!$A$1:$H$1</definedName></definedNames><calcPr calcId="124519" fullCalcOnLoad="true"/></workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -995,4 +983,61 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row outlineLevel="0" r="1">
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" s="0" t="inlineStr">
+        <is>
+          <t>gender</t>
+        </is>
+      </c>
+      <c r="D1" s="0" t="inlineStr">
+        <is>
+          <t>age</t>
+        </is>
+      </c>
+      <c r="E1" s="0" t="inlineStr">
+        <is>
+          <t>salary</t>
+        </is>
+      </c>
+      <c r="F1" s="0" t="inlineStr">
+        <is>
+          <t>dept</t>
+        </is>
+      </c>
+      <c r="G1" s="0" t="inlineStr">
+        <is>
+          <t>deptno</t>
+        </is>
+      </c>
+      <c r="H1" s="0" t="inlineStr">
+        <is>
+          <t>doj</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>